<commit_message>
updated measures and weights for 2013-2025 version
</commit_message>
<xml_diff>
--- a/data/temp/measures.xlsx
+++ b/data/temp/measures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hardws/Documents/us_tariffs/data/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D0604C-5A95-564E-884E-65040600E14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585B2F96-2595-DB4F-902B-279EF1E3AD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1227,10 +1227,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V100"/>
+  <dimension ref="A1:V99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5271,6 +5272,8 @@
       <c r="V90" s="3"/>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="I91"/>
+      <c r="J91"/>
       <c r="Q91" s="3"/>
       <c r="R91" s="3"/>
       <c r="S91" s="3"/>
@@ -5278,8 +5281,8 @@
       <c r="V91" s="3"/>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="I92"/>
-      <c r="J92"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
       <c r="Q92" s="3"/>
       <c r="R92" s="3"/>
       <c r="S92" s="3"/>
@@ -5307,11 +5310,6 @@
     <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
-      <c r="Q95" s="3"/>
-      <c r="R95" s="3"/>
-      <c r="S95" s="3"/>
-      <c r="U95" s="3"/>
-      <c r="V95" s="3"/>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="I96" s="3"/>
@@ -5328,10 +5326,6 @@
     <row r="99" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
-    </row>
-    <row r="100" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P85" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>